<commit_message>
Updated and reworked PTMViz tool
</commit_message>
<xml_diff>
--- a/Data/PTMViz Metadata.xlsx
+++ b/Data/PTMViz Metadata.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmcha\OneDrive\Documents\GitHub\PTMViz\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin Chappell\Documents\GitHub\PTMViz\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{61029946-7DF0-4946-95F1-EB967247B922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DB722C-82F0-44BD-8AB4-6B2A92F9CD08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="18224" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="67">
   <si>
     <t>Proteins:</t>
   </si>
@@ -588,19 +589,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1328125" customWidth="1"/>
-    <col min="3" max="3" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.59765625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -646,7 +647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -684,7 +685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -722,7 +723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -760,7 +761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -798,7 +799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -836,7 +837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -874,7 +875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>9</v>
       </c>
@@ -900,7 +901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>9</v>
       </c>
@@ -926,7 +927,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
       <c r="F12" t="s">
         <v>9</v>
       </c>
@@ -952,7 +965,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
       <c r="F13" t="s">
         <v>9</v>
       </c>
@@ -978,7 +1003,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
       <c r="F14" t="s">
         <v>9</v>
       </c>
@@ -1004,7 +1041,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
@@ -1030,7 +1079,35 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1044,7 +1121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>21</v>
       </c>
@@ -1058,7 +1135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>21</v>
       </c>
@@ -1072,7 +1149,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>21</v>
       </c>
@@ -1086,7 +1163,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>21</v>
       </c>
@@ -1100,7 +1177,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>21</v>
       </c>
@@ -1114,7 +1191,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>21</v>
       </c>
@@ -1128,7 +1205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>21</v>
       </c>
@@ -1142,7 +1219,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>21</v>
       </c>
@@ -1156,7 +1233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>21</v>
       </c>
@@ -1170,7 +1247,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>21</v>
       </c>
@@ -1184,7 +1261,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>21</v>
       </c>
@@ -1198,7 +1275,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>21</v>
       </c>
@@ -1212,7 +1289,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
         <v>24</v>
       </c>
@@ -1226,7 +1303,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>24</v>
       </c>
@@ -1240,7 +1317,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>24</v>
       </c>
@@ -1254,7 +1331,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>24</v>
       </c>
@@ -1268,7 +1345,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
         <v>24</v>
       </c>
@@ -1282,7 +1359,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
         <v>24</v>
       </c>
@@ -1296,7 +1373,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1387,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>24</v>
       </c>
@@ -1324,7 +1401,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1415,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>24</v>
       </c>
@@ -1352,7 +1429,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>24</v>
       </c>
@@ -1366,7 +1443,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>24</v>
       </c>
@@ -1380,7 +1457,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
         <v>25</v>
       </c>
@@ -1394,7 +1471,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
         <v>25</v>
       </c>
@@ -1408,7 +1485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>25</v>
       </c>
@@ -1422,7 +1499,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>25</v>
       </c>
@@ -1436,7 +1513,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
         <v>25</v>
       </c>
@@ -1450,7 +1527,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
         <v>25</v>
       </c>
@@ -1464,7 +1541,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
         <v>25</v>
       </c>
@@ -1478,7 +1555,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
         <v>25</v>
       </c>
@@ -1492,7 +1569,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
         <v>25</v>
       </c>
@@ -1506,7 +1583,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
         <v>25</v>
       </c>
@@ -1520,7 +1597,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
         <v>25</v>
       </c>
@@ -1534,7 +1611,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="6:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
         <v>25</v>
       </c>

</xml_diff>